<commit_message>
read old excel and write to new excel with preprocessed exp
</commit_message>
<xml_diff>
--- a/python_script_preprocessing/Inputtypesfilesspreadsheet.xlsx
+++ b/python_script_preprocessing/Inputtypesfilesspreadsheet.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arithmethic-parser-\python_script_preprocessing\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBAD5B1-6F32-4F45-9DE9-CA84177470A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0" calcOnSave="0"/>
 </workbook>
 </file>
 
@@ -16,12 +25,6 @@
     <t>Input</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>output</t>
-  </si>
-  <si>
     <t>current compileing</t>
   </si>
   <si>
@@ -575,36 +578,42 @@
   </si>
   <si>
     <t>Fraction(2001001001000000000000001001, 1000000000000000000000000000)</t>
+  </si>
+  <si>
+    <t>Preprocessed expression</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GUI output</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color rgb="FFFFFFFF"/>
       <name val="Algerian"/>
     </font>
     <font>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Algerian"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="&quot;Times New Roman&quot;"/>
     </font>
@@ -614,7 +623,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -654,83 +663,63 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="22">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf quotePrefix="1" borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -920,36 +909,42 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I93"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="23.29"/>
-    <col customWidth="1" min="3" max="3" width="44.29"/>
-    <col customWidth="1" min="4" max="4" width="47.57"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="38.21875" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" customWidth="1"/>
+    <col min="4" max="4" width="47.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -957,16 +952,16 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1">
       <c r="A2" s="4">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -974,16 +969,16 @@
       <c r="H2" s="7"/>
       <c r="I2" s="8"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -991,16 +986,16 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -1008,16 +1003,16 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1">
       <c r="A5" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -1025,16 +1020,16 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:9" ht="15.75" customHeight="1">
       <c r="A6" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -1042,16 +1037,16 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:9" ht="15.75" customHeight="1">
       <c r="A7" s="9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -1059,16 +1054,16 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:9" ht="15.75" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -1076,16 +1071,16 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:9" ht="15.75" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -1093,13 +1088,13 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:9" ht="15.75" customHeight="1">
       <c r="A10" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -1108,13 +1103,13 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:9" ht="15.75" customHeight="1">
       <c r="A11" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -1123,13 +1118,13 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:9" ht="15.75" customHeight="1">
       <c r="A12" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -1138,13 +1133,13 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:9" ht="15.75" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -1153,13 +1148,13 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:9" ht="15.75" customHeight="1">
       <c r="A14" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -1168,16 +1163,16 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:9" ht="15.75" customHeight="1">
       <c r="A15" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -1185,16 +1180,16 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:9" ht="15.75" customHeight="1">
       <c r="A16" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -1202,13 +1197,13 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:9" ht="15.75" customHeight="1">
       <c r="A17" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -1217,16 +1212,16 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:9" ht="15.75" customHeight="1">
       <c r="A18" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -1234,16 +1229,16 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:9" ht="15.75" customHeight="1">
       <c r="A19" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -1251,16 +1246,16 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:9" ht="15.75" customHeight="1">
       <c r="A20" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -1268,16 +1263,16 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:9" ht="15.75" customHeight="1">
       <c r="A21" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -1285,16 +1280,16 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:9" ht="15.75" customHeight="1">
       <c r="A22" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -1302,16 +1297,16 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:9" ht="15.75" customHeight="1">
       <c r="A23" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -1319,16 +1314,16 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:9" ht="15.75" customHeight="1">
       <c r="A24" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -1336,16 +1331,16 @@
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:9" ht="15.75" customHeight="1">
       <c r="A25" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -1353,16 +1348,16 @@
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:9" ht="15.75" customHeight="1">
       <c r="A26" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -1370,16 +1365,16 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:9" ht="14.4">
       <c r="A27" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -1387,16 +1382,16 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:9" ht="14.4">
       <c r="A28" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -1404,16 +1399,16 @@
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:9" ht="14.4">
       <c r="A29" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B29" s="10"/>
       <c r="C29" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -1421,16 +1416,16 @@
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:9" ht="14.4">
       <c r="A30" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -1438,18 +1433,18 @@
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:9" ht="14.4">
       <c r="A31" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="D31" s="14" t="s">
         <v>57</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>59</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -1457,16 +1452,16 @@
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:9" ht="14.4">
       <c r="A32" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B32" s="10"/>
       <c r="C32" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
@@ -1474,16 +1469,16 @@
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:9" ht="14.4">
       <c r="A33" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B33" s="10"/>
       <c r="C33" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -1491,16 +1486,16 @@
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:9" ht="14.4">
       <c r="A34" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B34" s="10"/>
       <c r="C34" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
@@ -1508,16 +1503,16 @@
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:9" ht="14.4">
       <c r="A35" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B35" s="15"/>
       <c r="C35" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
@@ -1525,16 +1520,16 @@
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:9" ht="14.4">
       <c r="A36" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B36" s="15"/>
       <c r="C36" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
@@ -1542,16 +1537,16 @@
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:9" ht="14.4">
       <c r="A37" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B37" s="15"/>
       <c r="C37" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D37" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
@@ -1559,13 +1554,13 @@
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:9" ht="14.4">
       <c r="A38" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B38" s="15"/>
       <c r="C38" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
@@ -1574,13 +1569,13 @@
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:9" ht="14.4">
       <c r="A39" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
@@ -1589,16 +1584,16 @@
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:9" ht="14.4">
       <c r="A40" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B40" s="15"/>
       <c r="C40" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
@@ -1606,16 +1601,16 @@
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
     </row>
-    <row r="41">
+    <row r="41" spans="1:9" ht="14.4">
       <c r="A41" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B41" s="10"/>
       <c r="C41" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D41" s="7" t="s">
         <v>77</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
@@ -1623,16 +1618,16 @@
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
     </row>
-    <row r="42">
+    <row r="42" spans="1:9" ht="14.4">
       <c r="A42" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B42" s="10"/>
       <c r="C42" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
@@ -1640,18 +1635,18 @@
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
     </row>
-    <row r="43">
+    <row r="43" spans="1:9" ht="14.4">
       <c r="A43" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B43" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>84</v>
-      </c>
       <c r="D43" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
@@ -1659,18 +1654,18 @@
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
     </row>
-    <row r="44">
+    <row r="44" spans="1:9" ht="14.4">
       <c r="A44" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B44" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>87</v>
-      </c>
       <c r="D44" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
@@ -1678,16 +1673,16 @@
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
     </row>
-    <row r="45">
+    <row r="45" spans="1:9" ht="14.4">
       <c r="A45" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B45" s="10"/>
       <c r="C45" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
@@ -1695,13 +1690,13 @@
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
     </row>
-    <row r="46">
+    <row r="46" spans="1:9" ht="14.4">
       <c r="A46" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B46" s="10"/>
       <c r="C46" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
@@ -1710,13 +1705,13 @@
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
     </row>
-    <row r="47">
+    <row r="47" spans="1:9" ht="14.4">
       <c r="A47" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
@@ -1725,13 +1720,13 @@
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
     </row>
-    <row r="48">
+    <row r="48" spans="1:9" ht="14.4">
       <c r="A48" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B48" s="10"/>
       <c r="C48" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
@@ -1740,13 +1735,13 @@
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
     </row>
-    <row r="49">
+    <row r="49" spans="1:9" ht="14.4">
       <c r="A49" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B49" s="10"/>
       <c r="C49" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
@@ -1755,15 +1750,15 @@
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
     </row>
-    <row r="50">
+    <row r="50" spans="1:9" ht="14.4">
       <c r="A50" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C50" s="7" t="s">
         <v>98</v>
-      </c>
-      <c r="B50" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>100</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
@@ -1772,15 +1767,15 @@
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
     </row>
-    <row r="51">
+    <row r="51" spans="1:9" ht="14.4">
       <c r="A51" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
@@ -1789,15 +1784,15 @@
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
     </row>
-    <row r="52">
+    <row r="52" spans="1:9" ht="14.4">
       <c r="A52" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
@@ -1806,15 +1801,15 @@
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
     </row>
-    <row r="53">
+    <row r="53" spans="1:9" ht="14.4">
       <c r="A53" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
@@ -1823,18 +1818,18 @@
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
     </row>
-    <row r="54">
+    <row r="54" spans="1:9" ht="14.4">
       <c r="A54" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C54" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B54" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>109</v>
-      </c>
       <c r="D54" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
@@ -1842,18 +1837,18 @@
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
     </row>
-    <row r="55">
+    <row r="55" spans="1:9" ht="14.4">
       <c r="A55" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C55" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B55" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>112</v>
-      </c>
       <c r="D55" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
@@ -1861,13 +1856,13 @@
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
     </row>
-    <row r="56">
+    <row r="56" spans="1:9" ht="14.4">
       <c r="A56" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B56" s="10"/>
       <c r="C56" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
@@ -1876,13 +1871,13 @@
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
     </row>
-    <row r="57">
+    <row r="57" spans="1:9" ht="14.4">
       <c r="A57" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B57" s="10"/>
       <c r="C57" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
@@ -1891,13 +1886,13 @@
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
     </row>
-    <row r="58">
+    <row r="58" spans="1:9" ht="14.4">
       <c r="A58" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
@@ -1906,13 +1901,13 @@
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
     </row>
-    <row r="59">
+    <row r="59" spans="1:9" ht="14.4">
       <c r="A59" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B59" s="10"/>
       <c r="C59" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
@@ -1921,13 +1916,13 @@
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
     </row>
-    <row r="60">
+    <row r="60" spans="1:9" ht="14.4">
       <c r="A60" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B60" s="10"/>
       <c r="C60" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
@@ -1936,13 +1931,13 @@
       <c r="H60" s="3"/>
       <c r="I60" s="3"/>
     </row>
-    <row r="61">
+    <row r="61" spans="1:9" ht="14.4">
       <c r="A61" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B61" s="10"/>
       <c r="C61" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
@@ -1951,13 +1946,13 @@
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
     </row>
-    <row r="62">
+    <row r="62" spans="1:9" ht="14.4">
       <c r="A62" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B62" s="10"/>
       <c r="C62" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
@@ -1966,13 +1961,13 @@
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
     </row>
-    <row r="63">
+    <row r="63" spans="1:9" ht="14.4">
       <c r="A63" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B63" s="10"/>
       <c r="C63" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
@@ -1981,13 +1976,13 @@
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
     </row>
-    <row r="64">
+    <row r="64" spans="1:9" ht="14.4">
       <c r="A64" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B64" s="10"/>
       <c r="C64" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
@@ -1996,13 +1991,13 @@
       <c r="H64" s="3"/>
       <c r="I64" s="3"/>
     </row>
-    <row r="65">
+    <row r="65" spans="1:9" ht="14.4">
       <c r="A65" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B65" s="10"/>
       <c r="C65" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
@@ -2011,13 +2006,13 @@
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
     </row>
-    <row r="66">
+    <row r="66" spans="1:9" ht="14.4">
       <c r="A66" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B66" s="10"/>
       <c r="C66" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
@@ -2026,13 +2021,13 @@
       <c r="H66" s="3"/>
       <c r="I66" s="3"/>
     </row>
-    <row r="67">
+    <row r="67" spans="1:9" ht="14.4">
       <c r="A67" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B67" s="10"/>
       <c r="C67" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
@@ -2041,13 +2036,13 @@
       <c r="H67" s="3"/>
       <c r="I67" s="3"/>
     </row>
-    <row r="68">
+    <row r="68" spans="1:9" ht="14.4">
       <c r="A68" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B68" s="10"/>
       <c r="C68" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
@@ -2056,13 +2051,13 @@
       <c r="H68" s="3"/>
       <c r="I68" s="3"/>
     </row>
-    <row r="69">
+    <row r="69" spans="1:9" ht="14.4">
       <c r="A69" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B69" s="10"/>
       <c r="C69" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
@@ -2071,13 +2066,13 @@
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
     </row>
-    <row r="70">
+    <row r="70" spans="1:9" ht="14.4">
       <c r="A70" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B70" s="10"/>
       <c r="C70" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
@@ -2086,13 +2081,13 @@
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
     </row>
-    <row r="71">
+    <row r="71" spans="1:9" ht="14.4">
       <c r="A71" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B71" s="10"/>
       <c r="C71" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
@@ -2101,13 +2096,13 @@
       <c r="H71" s="3"/>
       <c r="I71" s="3"/>
     </row>
-    <row r="72">
+    <row r="72" spans="1:9" ht="14.4">
       <c r="A72" s="9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B72" s="10"/>
       <c r="C72" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
@@ -2116,13 +2111,13 @@
       <c r="H72" s="3"/>
       <c r="I72" s="3"/>
     </row>
-    <row r="73">
+    <row r="73" spans="1:9" ht="14.4">
       <c r="A73" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B73" s="10"/>
       <c r="C73" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
@@ -2131,15 +2126,15 @@
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
     </row>
-    <row r="74">
+    <row r="74" spans="1:9" ht="14.4">
       <c r="A74" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B74" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="C74" s="7" t="s">
         <v>148</v>
-      </c>
-      <c r="B74" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>150</v>
       </c>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
@@ -2148,35 +2143,43 @@
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
     </row>
-    <row r="75">
-      <c r="A75" s="9" t="s">
+    <row r="75" spans="1:9" ht="14.4">
+      <c r="A75" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="B75" s="20"/>
+      <c r="C75" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="D75" s="20"/>
+      <c r="E75" s="20"/>
+      <c r="F75" s="20"/>
+      <c r="G75" s="20"/>
+      <c r="H75" s="20"/>
+      <c r="I75" s="3"/>
+    </row>
+    <row r="76" spans="1:9" ht="14.4">
+      <c r="A76" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="C75" s="7" t="s">
+      <c r="B76" s="20"/>
+      <c r="C76" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="I75" s="3"/>
-    </row>
-    <row r="76">
-      <c r="A76" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="C76" s="7" t="s">
-        <v>154</v>
-      </c>
+      <c r="D76" s="20"/>
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
       <c r="I76" s="3"/>
     </row>
-    <row r="77">
+    <row r="77" spans="1:9" ht="14.4">
       <c r="A77" s="9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B77" s="10"/>
       <c r="C77" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
@@ -2185,29 +2188,30 @@
       <c r="H77" s="3"/>
       <c r="I77" s="3"/>
     </row>
-    <row r="78">
+    <row r="78" spans="1:9" ht="14.4">
       <c r="A78" s="9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B78" s="10"/>
-      <c r="C78" s="7" t="s">
-        <v>158</v>
-      </c>
+      <c r="C78" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="D78" s="20"/>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
       <c r="I78" s="3"/>
     </row>
-    <row r="79">
+    <row r="79" spans="1:9" ht="14.4">
       <c r="A79" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B79" s="17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
@@ -2216,13 +2220,13 @@
       <c r="H79" s="3"/>
       <c r="I79" s="3"/>
     </row>
-    <row r="80">
+    <row r="80" spans="1:9" ht="14.4">
       <c r="A80" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B80" s="10"/>
       <c r="C80" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
@@ -2231,13 +2235,13 @@
       <c r="H80" s="3"/>
       <c r="I80" s="3"/>
     </row>
-    <row r="81">
+    <row r="81" spans="1:9" ht="14.4">
       <c r="A81" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B81" s="10"/>
       <c r="C81" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
@@ -2246,13 +2250,13 @@
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
     </row>
-    <row r="82">
+    <row r="82" spans="1:9" ht="14.4">
       <c r="A82" s="9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B82" s="10"/>
       <c r="C82" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D82" s="3"/>
       <c r="E82" s="3"/>
@@ -2261,13 +2265,13 @@
       <c r="H82" s="3"/>
       <c r="I82" s="3"/>
     </row>
-    <row r="83">
+    <row r="83" spans="1:9" ht="14.4">
       <c r="A83" s="9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B83" s="10"/>
       <c r="C83" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
@@ -2276,13 +2280,13 @@
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
     </row>
-    <row r="84">
+    <row r="84" spans="1:9" ht="14.4">
       <c r="A84" s="9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B84" s="10"/>
       <c r="C84" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
@@ -2291,13 +2295,13 @@
       <c r="H84" s="3"/>
       <c r="I84" s="3"/>
     </row>
-    <row r="85">
+    <row r="85" spans="1:9" ht="14.4">
       <c r="A85" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B85" s="10"/>
       <c r="C85" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
@@ -2306,13 +2310,13 @@
       <c r="H85" s="3"/>
       <c r="I85" s="3"/>
     </row>
-    <row r="86">
+    <row r="86" spans="1:9" ht="14.4">
       <c r="A86" s="9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B86" s="10"/>
       <c r="C86" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
@@ -2321,13 +2325,13 @@
       <c r="H86" s="3"/>
       <c r="I86" s="3"/>
     </row>
-    <row r="87">
+    <row r="87" spans="1:9" ht="14.4">
       <c r="A87" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B87" s="10"/>
       <c r="C87" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
@@ -2336,13 +2340,13 @@
       <c r="H87" s="3"/>
       <c r="I87" s="3"/>
     </row>
-    <row r="88">
+    <row r="88" spans="1:9" ht="14.4">
       <c r="A88" s="9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B88" s="10"/>
       <c r="C88" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
@@ -2351,13 +2355,13 @@
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
     </row>
-    <row r="89">
+    <row r="89" spans="1:9" ht="14.4">
       <c r="A89" s="9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B89" s="10"/>
       <c r="C89" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
@@ -2366,13 +2370,13 @@
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
     </row>
-    <row r="90">
+    <row r="90" spans="1:9" ht="14.4">
       <c r="A90" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B90" s="10"/>
       <c r="C90" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
@@ -2381,13 +2385,13 @@
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
     </row>
-    <row r="91">
+    <row r="91" spans="1:9" ht="14.4">
       <c r="A91" s="9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B91" s="10"/>
       <c r="C91" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
@@ -2396,13 +2400,13 @@
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
     </row>
-    <row r="92">
+    <row r="92" spans="1:9" ht="14.4">
       <c r="A92" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B92" s="10"/>
       <c r="C92" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
@@ -2411,13 +2415,13 @@
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
     </row>
-    <row r="93">
+    <row r="93" spans="1:9" ht="14.4">
       <c r="A93" s="9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B93" s="10"/>
       <c r="C93" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
@@ -2434,6 +2438,6 @@
     <mergeCell ref="C76:D76"/>
     <mergeCell ref="C78:D78"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
compare columns of ap and cparsed op
</commit_message>
<xml_diff>
--- a/python_script_preprocessing/Inputtypesfilesspreadsheet.xlsx
+++ b/python_script_preprocessing/Inputtypesfilesspreadsheet.xlsx
@@ -8,26 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arithmethic-parser-\python_script_preprocessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CA96B2-C29A-4CF4-AE79-0561F8AB712E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E44A0D-6327-4E62-A874-8ED341C9668C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="263">
   <si>
     <t>Input</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
     <t>output</t>
   </si>
   <si>
@@ -193,9 +190,6 @@
     <t>-5p/-2k+(8M/5m)*2n'</t>
   </si>
   <si>
-    <t>-(5*p)/-(2*k)+((8*M)/(5*m)*(2*n)'</t>
-  </si>
-  <si>
     <t>Fraction(1280000000000001, 400000000000000)</t>
   </si>
   <si>
@@ -271,18 +265,12 @@
     <t>0.8u*1e10'</t>
   </si>
   <si>
-    <t>(0.8*u)*1e10'</t>
-  </si>
-  <si>
     <t>Fraction(80000, 1)</t>
   </si>
   <si>
     <t>((.9M*.1m-.10+6da))/(.1)</t>
   </si>
   <si>
-    <t>(((.9*M)*(.1*m)-.10+(6*da)))/(.1)</t>
-  </si>
-  <si>
     <t>Fraction(1499, 1)</t>
   </si>
   <si>
@@ -319,9 +307,6 @@
     <t>909m+345n+1T*1z</t>
   </si>
   <si>
-    <t>INVALID</t>
-  </si>
-  <si>
     <t>Fraction(454500173, 500000000)</t>
   </si>
   <si>
@@ -346,18 +331,12 @@
     <t>899G*1u+1e3-16e4</t>
   </si>
   <si>
-    <t>(899*G)*(1*u)+(1e3-16e4)</t>
-  </si>
-  <si>
     <t>Fraction(740000, 1)</t>
   </si>
   <si>
     <t>0.124P*0.1u+1e3-16e4'</t>
   </si>
   <si>
-    <t>(0.124*P)*(0.1*u)+(1e3-16e4)</t>
-  </si>
-  <si>
     <t>Fraction(12241000, 1)</t>
   </si>
   <si>
@@ -469,9 +448,6 @@
     <t>(9u/43M/56c/67h/300E/15e-8)*1e34</t>
   </si>
   <si>
-    <t>Above power20</t>
-  </si>
-  <si>
     <t>Fraction(250000000, 20167)</t>
   </si>
   <si>
@@ -596,13 +572,250 @@
   </si>
   <si>
     <t>5+G</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>4/5</t>
+  </si>
+  <si>
+    <t>20000000</t>
+  </si>
+  <si>
+    <t>1001/50</t>
+  </si>
+  <si>
+    <t>999/50</t>
+  </si>
+  <si>
+    <t>2/5</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>19001/1000</t>
+  </si>
+  <si>
+    <t>4000000</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>57/10</t>
+  </si>
+  <si>
+    <t>6400005/2</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>121/2</t>
+  </si>
+  <si>
+    <t>1280000000000001/400000000000000</t>
+  </si>
+  <si>
+    <t>1430511474609374976/476837158203125</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>59604644775390625/6622738308376736</t>
+  </si>
+  <si>
+    <t>1490116119384765625/1655684577094184</t>
+  </si>
+  <si>
+    <t>1862647218836678398980/206960572136773</t>
+  </si>
+  <si>
+    <t>112234563/8989000</t>
+  </si>
+  <si>
+    <t>112234563000/8989</t>
+  </si>
+  <si>
+    <t>8000</t>
+  </si>
+  <si>
+    <t>1499</t>
+  </si>
+  <si>
+    <t>2002000</t>
+  </si>
+  <si>
+    <t>101000</t>
+  </si>
+  <si>
+    <t>300700021/700</t>
+  </si>
+  <si>
+    <t>26666666666666666219274239989/47619047619047618248704</t>
+  </si>
+  <si>
+    <t>69710923/125</t>
+  </si>
+  <si>
+    <t>454500173/500000000</t>
+  </si>
+  <si>
+    <t>1000000089/1000000</t>
+  </si>
+  <si>
+    <t>2000000000000000000000899/2000000000000000000</t>
+  </si>
+  <si>
+    <t>899</t>
+  </si>
+  <si>
+    <t>740000</t>
+  </si>
+  <si>
+    <t>12241000</t>
+  </si>
+  <si>
+    <t>58497007500000008500000000019/250000000000000000000</t>
+  </si>
+  <si>
+    <t>81250000/323</t>
+  </si>
+  <si>
+    <t>18609254</t>
+  </si>
+  <si>
+    <t>8350983000000823/1000000000</t>
+  </si>
+  <si>
+    <t>7878208/207</t>
+  </si>
+  <si>
+    <t>19217447916666666344229907625/325520833333333327872</t>
+  </si>
+  <si>
+    <t>1356499948847/59000000000</t>
+  </si>
+  <si>
+    <t>117493861407/500000000</t>
+  </si>
+  <si>
+    <t>40177035847845530971216489/2838316417875744000</t>
+  </si>
+  <si>
+    <t>38960000</t>
+  </si>
+  <si>
+    <t>25200000</t>
+  </si>
+  <si>
+    <t>252000</t>
+  </si>
+  <si>
+    <t>5836251091/250</t>
+  </si>
+  <si>
+    <t>51/80</t>
+  </si>
+  <si>
+    <t>8600000111999999397/200000000000</t>
+  </si>
+  <si>
+    <t>19350000252004049933/450000000000</t>
+  </si>
+  <si>
+    <t>250000000/20167</t>
+  </si>
+  <si>
+    <t>10007090001/1000</t>
+  </si>
+  <si>
+    <t>33321343000000000000000000000000501/18139000000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>20694807/25000</t>
+  </si>
+  <si>
+    <t>1250000000/15219</t>
+  </si>
+  <si>
+    <t>9131400/7</t>
+  </si>
+  <si>
+    <t>620521300178000000011/2000000000000000000</t>
+  </si>
+  <si>
+    <t>33163200000000000006853/160000000000000</t>
+  </si>
+  <si>
+    <t>82908000000267267/40000000000000</t>
+  </si>
+  <si>
+    <t>26800000000012727/400000000</t>
+  </si>
+  <si>
+    <t>800011/200</t>
+  </si>
+  <si>
+    <t>24500000000000001/25000000000000000</t>
+  </si>
+  <si>
+    <t>175000002449825001/25000000000000</t>
+  </si>
+  <si>
+    <t>80078400000000000000000000000079/10000000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>1000000000001001/1000000000</t>
+  </si>
+  <si>
+    <t>6001010001000001003001/1000000000000000</t>
+  </si>
+  <si>
+    <t>8000000200201/200000000000</t>
+  </si>
+  <si>
+    <t>2001001001000000000000001001/1000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>1201/20</t>
+  </si>
+  <si>
+    <t>66605209/500000</t>
+  </si>
+  <si>
+    <t>Arithmetic parser op</t>
+  </si>
+  <si>
+    <t>Preprocessed exp</t>
+  </si>
+  <si>
+    <t>cparsed op</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -629,8 +842,13 @@
       <color rgb="FF000000"/>
       <name val="&quot;Times New Roman&quot;"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -657,20 +875,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor rgb="FFFFC000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FFFF0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor rgb="FF00B050"/>
       </patternFill>
     </fill>
   </fills>
@@ -686,15 +892,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -707,9 +910,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -933,13 +1135,14 @@
   </sheetPr>
   <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="16"/>
     <col min="3" max="3" width="44.33203125" customWidth="1"/>
     <col min="4" max="4" width="47.5546875" customWidth="1"/>
   </cols>
@@ -949,16 +1152,20 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="E1" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>262</v>
+      </c>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -967,29 +1174,33 @@
       <c r="A2" s="4">
         <v>20</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>4</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>5</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="8"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="7"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -999,14 +1210,16 @@
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1">
       <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>8</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>9</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -1015,15 +1228,17 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>11</v>
+      <c r="D5" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -1032,15 +1247,17 @@
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -1049,15 +1266,17 @@
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>16</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -1066,15 +1285,17 @@
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>18</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -1084,14 +1305,16 @@
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>18</v>
+      <c r="B9" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -1100,12 +1323,14 @@
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="7" t="s">
-        <v>21</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -1115,12 +1340,14 @@
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="7" t="s">
-        <v>23</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -1130,12 +1357,14 @@
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="7" t="s">
-        <v>25</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -1145,12 +1374,14 @@
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="7" t="s">
-        <v>27</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -1160,12 +1391,14 @@
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A14" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="7" t="s">
+      <c r="A14" s="8" t="s">
         <v>27</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -1175,15 +1408,17 @@
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>30</v>
+      <c r="D15" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -1192,15 +1427,17 @@
       <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>32</v>
+      <c r="D16" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -1209,12 +1446,14 @@
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A17" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="7" t="s">
+      <c r="A17" s="8" t="s">
         <v>27</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -1224,15 +1463,17 @@
       <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A18" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="6" t="s">
+      <c r="A18" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>32</v>
+      <c r="B18" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -1241,15 +1482,17 @@
       <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>35</v>
+      <c r="D19" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -1258,15 +1501,17 @@
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A20" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="12" t="s">
+      <c r="A20" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="13" t="s">
-        <v>35</v>
+      <c r="B20" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>34</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -1275,15 +1520,17 @@
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>38</v>
+      <c r="D21" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -1292,15 +1539,17 @@
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A22" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="6" t="s">
+      <c r="A22" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>38</v>
+      <c r="B22" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -1309,15 +1558,17 @@
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="6" t="s">
+      <c r="D23" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>42</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -1326,15 +1577,17 @@
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="7" t="s">
+      <c r="D24" s="13" t="s">
         <v>44</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>45</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -1343,15 +1596,17 @@
       <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A25" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>46</v>
+      <c r="A25" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -1360,15 +1615,17 @@
       <c r="I25" s="3"/>
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>48</v>
+      <c r="D26" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -1377,15 +1634,17 @@
       <c r="I26" s="3"/>
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A27" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>44</v>
+      <c r="A27" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -1394,15 +1653,17 @@
       <c r="I27" s="3"/>
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A28" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>44</v>
+      <c r="A28" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -1411,15 +1672,17 @@
       <c r="I28" s="3"/>
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="7" t="s">
+      <c r="D29" s="13" t="s">
         <v>52</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>53</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -1428,15 +1691,17 @@
       <c r="I29" s="3"/>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>53</v>
+      <c r="D30" s="13" t="s">
+        <v>52</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -1445,17 +1710,17 @@
       <c r="I30" s="3"/>
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="D31" s="13" t="s">
         <v>57</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>59</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -1464,15 +1729,17 @@
       <c r="I31" s="3"/>
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A32" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" s="10"/>
-      <c r="C32" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>41</v>
+      <c r="A32" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
@@ -1481,15 +1748,17 @@
       <c r="I32" s="3"/>
     </row>
     <row r="33" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="13" t="s">
         <v>61</v>
-      </c>
-      <c r="B33" s="10"/>
-      <c r="C33" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>63</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -1498,15 +1767,17 @@
       <c r="I33" s="3"/>
     </row>
     <row r="34" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A34" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" s="10"/>
-      <c r="C34" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>65</v>
+      <c r="A34" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
@@ -1515,15 +1786,17 @@
       <c r="I34" s="3"/>
     </row>
     <row r="35" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A35" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35" s="15"/>
-      <c r="C35" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>53</v>
+      <c r="A35" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>52</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
@@ -1532,15 +1805,17 @@
       <c r="I35" s="3"/>
     </row>
     <row r="36" spans="1:9" ht="14.4">
-      <c r="A36" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B36" s="15"/>
-      <c r="C36" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>53</v>
+      <c r="A36" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>52</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
@@ -1549,15 +1824,17 @@
       <c r="I36" s="3"/>
     </row>
     <row r="37" spans="1:9" ht="14.4">
-      <c r="A37" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37" s="15"/>
-      <c r="C37" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>53</v>
+      <c r="A37" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>52</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
@@ -1566,12 +1843,14 @@
       <c r="I37" s="3"/>
     </row>
     <row r="38" spans="1:9" ht="14.4">
-      <c r="A38" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B38" s="15"/>
-      <c r="C38" s="7" t="s">
-        <v>73</v>
+      <c r="A38" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
@@ -1581,12 +1860,14 @@
       <c r="I38" s="3"/>
     </row>
     <row r="39" spans="1:9" ht="14.4">
-      <c r="A39" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B39" s="10"/>
-      <c r="C39" s="7" t="s">
-        <v>73</v>
+      <c r="A39" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
@@ -1596,15 +1877,17 @@
       <c r="I39" s="3"/>
     </row>
     <row r="40" spans="1:9" ht="14.4">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D40" s="13" t="s">
         <v>75</v>
-      </c>
-      <c r="B40" s="15"/>
-      <c r="C40" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D40" s="14" t="s">
-        <v>77</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
@@ -1613,15 +1896,17 @@
       <c r="I40" s="3"/>
     </row>
     <row r="41" spans="1:9" ht="14.4">
-      <c r="A41" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B41" s="10"/>
-      <c r="C41" s="7" t="s">
+      <c r="A41" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>77</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
@@ -1630,15 +1915,17 @@
       <c r="I41" s="3"/>
     </row>
     <row r="42" spans="1:9" ht="14.4">
-      <c r="A42" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B42" s="10"/>
-      <c r="C42" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D42" s="7" t="s">
+      <c r="A42" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="C42" s="6" t="s">
         <v>79</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>77</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
@@ -1647,17 +1934,17 @@
       <c r="I42" s="3"/>
     </row>
     <row r="43" spans="1:9" ht="14.4">
-      <c r="A43" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>84</v>
+      <c r="A43" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
@@ -1666,17 +1953,17 @@
       <c r="I43" s="3"/>
     </row>
     <row r="44" spans="1:9" ht="14.4">
-      <c r="A44" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>87</v>
+      <c r="A44" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>83</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
@@ -1685,15 +1972,17 @@
       <c r="I44" s="3"/>
     </row>
     <row r="45" spans="1:9" ht="14.4">
-      <c r="A45" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="B45" s="10"/>
-      <c r="C45" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>89</v>
+      <c r="A45" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
@@ -1702,12 +1991,14 @@
       <c r="I45" s="3"/>
     </row>
     <row r="46" spans="1:9" ht="14.4">
-      <c r="A46" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="B46" s="10"/>
-      <c r="C46" s="7" t="s">
-        <v>91</v>
+      <c r="A46" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
@@ -1717,12 +2008,14 @@
       <c r="I46" s="3"/>
     </row>
     <row r="47" spans="1:9" ht="14.4">
-      <c r="A47" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="B47" s="10"/>
-      <c r="C47" s="7" t="s">
-        <v>93</v>
+      <c r="A47" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>89</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
@@ -1732,12 +2025,14 @@
       <c r="I47" s="3"/>
     </row>
     <row r="48" spans="1:9" ht="14.4">
-      <c r="A48" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="B48" s="10"/>
-      <c r="C48" s="7" t="s">
-        <v>95</v>
+      <c r="A48" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>91</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
@@ -1747,12 +2042,14 @@
       <c r="I48" s="3"/>
     </row>
     <row r="49" spans="1:9" ht="14.4">
-      <c r="A49" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="B49" s="10"/>
-      <c r="C49" s="7" t="s">
-        <v>97</v>
+      <c r="A49" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
@@ -1762,14 +2059,14 @@
       <c r="I49" s="3"/>
     </row>
     <row r="50" spans="1:9" ht="14.4">
-      <c r="A50" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="B50" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>100</v>
+      <c r="A50" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
@@ -1779,14 +2076,14 @@
       <c r="I50" s="3"/>
     </row>
     <row r="51" spans="1:9" ht="14.4">
-      <c r="A51" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="B51" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>102</v>
+      <c r="A51" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>97</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
@@ -1796,14 +2093,14 @@
       <c r="I51" s="3"/>
     </row>
     <row r="52" spans="1:9" ht="14.4">
-      <c r="A52" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="B52" s="17" t="s">
+      <c r="A52" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="C52" s="6" t="s">
         <v>99</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
@@ -1813,14 +2110,14 @@
       <c r="I52" s="3"/>
     </row>
     <row r="53" spans="1:9" ht="14.4">
-      <c r="A53" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="B53" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>106</v>
+      <c r="A53" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>101</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
@@ -1830,17 +2127,17 @@
       <c r="I53" s="3"/>
     </row>
     <row r="54" spans="1:9" ht="14.4">
-      <c r="A54" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="B54" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>109</v>
+      <c r="A54" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B54" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>103</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
@@ -1849,17 +2146,17 @@
       <c r="I54" s="3"/>
     </row>
     <row r="55" spans="1:9" ht="14.4">
-      <c r="A55" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="B55" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>112</v>
+      <c r="A55" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B55" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>105</v>
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
@@ -1868,12 +2165,14 @@
       <c r="I55" s="3"/>
     </row>
     <row r="56" spans="1:9" ht="14.4">
-      <c r="A56" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="B56" s="10"/>
-      <c r="C56" s="7" t="s">
-        <v>114</v>
+      <c r="A56" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B56" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>107</v>
       </c>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
@@ -1883,12 +2182,14 @@
       <c r="I56" s="3"/>
     </row>
     <row r="57" spans="1:9" ht="14.4">
-      <c r="A57" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="B57" s="10"/>
-      <c r="C57" s="7" t="s">
-        <v>116</v>
+      <c r="A57" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
@@ -1898,12 +2199,14 @@
       <c r="I57" s="3"/>
     </row>
     <row r="58" spans="1:9" ht="14.4">
-      <c r="A58" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="B58" s="10"/>
-      <c r="C58" s="7" t="s">
-        <v>118</v>
+      <c r="A58" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B58" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>111</v>
       </c>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
@@ -1913,12 +2216,14 @@
       <c r="I58" s="3"/>
     </row>
     <row r="59" spans="1:9" ht="14.4">
-      <c r="A59" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="B59" s="10"/>
-      <c r="C59" s="7" t="s">
-        <v>120</v>
+      <c r="A59" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B59" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
@@ -1928,12 +2233,14 @@
       <c r="I59" s="3"/>
     </row>
     <row r="60" spans="1:9" ht="14.4">
-      <c r="A60" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="B60" s="10"/>
-      <c r="C60" s="7" t="s">
-        <v>122</v>
+      <c r="A60" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B60" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
@@ -1943,12 +2250,14 @@
       <c r="I60" s="3"/>
     </row>
     <row r="61" spans="1:9" ht="14.4">
-      <c r="A61" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="B61" s="10"/>
-      <c r="C61" s="7" t="s">
-        <v>124</v>
+      <c r="A61" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B61" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
@@ -1958,12 +2267,14 @@
       <c r="I61" s="3"/>
     </row>
     <row r="62" spans="1:9" ht="14.4">
-      <c r="A62" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="B62" s="10"/>
-      <c r="C62" s="7" t="s">
-        <v>126</v>
+      <c r="A62" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B62" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>119</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
@@ -1973,12 +2284,14 @@
       <c r="I62" s="3"/>
     </row>
     <row r="63" spans="1:9" ht="14.4">
-      <c r="A63" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="B63" s="10"/>
-      <c r="C63" s="7" t="s">
-        <v>128</v>
+      <c r="A63" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B63" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>121</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
@@ -1988,12 +2301,14 @@
       <c r="I63" s="3"/>
     </row>
     <row r="64" spans="1:9" ht="14.4">
-      <c r="A64" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="B64" s="10"/>
-      <c r="C64" s="7" t="s">
-        <v>129</v>
+      <c r="A64" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B64" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>122</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
@@ -2003,12 +2318,14 @@
       <c r="I64" s="3"/>
     </row>
     <row r="65" spans="1:9" ht="14.4">
-      <c r="A65" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="B65" s="10"/>
-      <c r="C65" s="7" t="s">
-        <v>131</v>
+      <c r="A65" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B65" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>124</v>
       </c>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
@@ -2018,12 +2335,14 @@
       <c r="I65" s="3"/>
     </row>
     <row r="66" spans="1:9" ht="14.4">
-      <c r="A66" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="B66" s="10"/>
-      <c r="C66" s="7" t="s">
-        <v>133</v>
+      <c r="A66" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B66" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>126</v>
       </c>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
@@ -2033,12 +2352,14 @@
       <c r="I66" s="3"/>
     </row>
     <row r="67" spans="1:9" ht="14.4">
-      <c r="A67" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="B67" s="10"/>
-      <c r="C67" s="7" t="s">
-        <v>135</v>
+      <c r="A67" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B67" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
@@ -2048,12 +2369,14 @@
       <c r="I67" s="3"/>
     </row>
     <row r="68" spans="1:9" ht="14.4">
-      <c r="A68" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="B68" s="10"/>
-      <c r="C68" s="7" t="s">
-        <v>137</v>
+      <c r="A68" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B68" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>130</v>
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
@@ -2063,12 +2386,14 @@
       <c r="I68" s="3"/>
     </row>
     <row r="69" spans="1:9" ht="14.4">
-      <c r="A69" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="B69" s="10"/>
-      <c r="C69" s="7" t="s">
-        <v>139</v>
+      <c r="A69" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B69" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>132</v>
       </c>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
@@ -2078,12 +2403,14 @@
       <c r="I69" s="3"/>
     </row>
     <row r="70" spans="1:9" ht="14.4">
-      <c r="A70" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B70" s="10"/>
-      <c r="C70" s="7" t="s">
-        <v>141</v>
+      <c r="A70" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B70" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>134</v>
       </c>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
@@ -2093,12 +2420,14 @@
       <c r="I70" s="3"/>
     </row>
     <row r="71" spans="1:9" ht="14.4">
-      <c r="A71" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B71" s="10"/>
-      <c r="C71" s="7" t="s">
-        <v>143</v>
+      <c r="A71" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B71" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>136</v>
       </c>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
@@ -2108,12 +2437,14 @@
       <c r="I71" s="3"/>
     </row>
     <row r="72" spans="1:9" ht="14.4">
-      <c r="A72" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="B72" s="10"/>
-      <c r="C72" s="7" t="s">
-        <v>145</v>
+      <c r="A72" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B72" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>138</v>
       </c>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
@@ -2123,12 +2454,14 @@
       <c r="I72" s="3"/>
     </row>
     <row r="73" spans="1:9" ht="14.4">
-      <c r="A73" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="B73" s="10"/>
-      <c r="C73" s="7" t="s">
-        <v>147</v>
+      <c r="A73" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B73" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>140</v>
       </c>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
@@ -2138,14 +2471,14 @@
       <c r="I73" s="3"/>
     </row>
     <row r="74" spans="1:9" ht="14.4">
-      <c r="A74" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="B74" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>150</v>
+      <c r="A74" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B74" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>142</v>
       </c>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
@@ -2155,29 +2488,29 @@
       <c r="I74" s="3"/>
     </row>
     <row r="75" spans="1:9" ht="14.4">
-      <c r="A75" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="B75" s="20"/>
-      <c r="C75" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="D75" s="20"/>
-      <c r="E75" s="20"/>
-      <c r="F75" s="20"/>
-      <c r="G75" s="20"/>
-      <c r="H75" s="20"/>
+      <c r="A75" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="B75" s="18"/>
+      <c r="C75" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="D75" s="18"/>
+      <c r="E75" s="18"/>
+      <c r="F75" s="18"/>
+      <c r="G75" s="18"/>
+      <c r="H75" s="18"/>
       <c r="I75" s="3"/>
     </row>
     <row r="76" spans="1:9" ht="14.4">
-      <c r="A76" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="B76" s="20"/>
-      <c r="C76" s="21" t="s">
-        <v>154</v>
-      </c>
-      <c r="D76" s="20"/>
+      <c r="A76" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="B76" s="18"/>
+      <c r="C76" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="D76" s="18"/>
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
@@ -2185,12 +2518,14 @@
       <c r="I76" s="3"/>
     </row>
     <row r="77" spans="1:9" ht="14.4">
-      <c r="A77" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="B77" s="10"/>
-      <c r="C77" s="7" t="s">
-        <v>156</v>
+      <c r="A77" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B77" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>148</v>
       </c>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
@@ -2200,14 +2535,16 @@
       <c r="I77" s="3"/>
     </row>
     <row r="78" spans="1:9" ht="14.4">
-      <c r="A78" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="B78" s="10"/>
-      <c r="C78" s="21" t="s">
-        <v>158</v>
-      </c>
-      <c r="D78" s="20"/>
+      <c r="A78" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B78" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="C78" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="D78" s="18"/>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
@@ -2215,14 +2552,14 @@
       <c r="I78" s="3"/>
     </row>
     <row r="79" spans="1:9" ht="14.4">
-      <c r="A79" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="B79" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>160</v>
+      <c r="A79" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B79" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>152</v>
       </c>
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
@@ -2232,12 +2569,14 @@
       <c r="I79" s="3"/>
     </row>
     <row r="80" spans="1:9" ht="14.4">
-      <c r="A80" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="B80" s="10"/>
-      <c r="C80" s="7" t="s">
-        <v>162</v>
+      <c r="A80" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B80" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>154</v>
       </c>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
@@ -2247,12 +2586,14 @@
       <c r="I80" s="3"/>
     </row>
     <row r="81" spans="1:9" ht="14.4">
-      <c r="A81" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="B81" s="10"/>
-      <c r="C81" s="7" t="s">
-        <v>164</v>
+      <c r="A81" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B81" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>156</v>
       </c>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
@@ -2262,12 +2603,14 @@
       <c r="I81" s="3"/>
     </row>
     <row r="82" spans="1:9" ht="14.4">
-      <c r="A82" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="B82" s="10"/>
-      <c r="C82" s="7" t="s">
-        <v>166</v>
+      <c r="A82" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B82" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>158</v>
       </c>
       <c r="D82" s="3"/>
       <c r="E82" s="3"/>
@@ -2277,12 +2620,14 @@
       <c r="I82" s="3"/>
     </row>
     <row r="83" spans="1:9" ht="14.4">
-      <c r="A83" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="B83" s="10"/>
-      <c r="C83" s="7" t="s">
-        <v>168</v>
+      <c r="A83" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B83" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>160</v>
       </c>
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
@@ -2292,12 +2637,14 @@
       <c r="I83" s="3"/>
     </row>
     <row r="84" spans="1:9" ht="14.4">
-      <c r="A84" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="B84" s="10"/>
-      <c r="C84" s="7" t="s">
-        <v>170</v>
+      <c r="A84" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B84" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>162</v>
       </c>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
@@ -2307,12 +2654,14 @@
       <c r="I84" s="3"/>
     </row>
     <row r="85" spans="1:9" ht="14.4">
-      <c r="A85" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="B85" s="10"/>
-      <c r="C85" s="7" t="s">
-        <v>172</v>
+      <c r="A85" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B85" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>164</v>
       </c>
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
@@ -2322,12 +2671,14 @@
       <c r="I85" s="3"/>
     </row>
     <row r="86" spans="1:9" ht="14.4">
-      <c r="A86" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="B86" s="10"/>
-      <c r="C86" s="7" t="s">
-        <v>174</v>
+      <c r="A86" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B86" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>166</v>
       </c>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
@@ -2337,12 +2688,14 @@
       <c r="I86" s="3"/>
     </row>
     <row r="87" spans="1:9" ht="14.4">
-      <c r="A87" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="B87" s="10"/>
-      <c r="C87" s="7" t="s">
-        <v>176</v>
+      <c r="A87" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B87" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>168</v>
       </c>
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
@@ -2352,12 +2705,14 @@
       <c r="I87" s="3"/>
     </row>
     <row r="88" spans="1:9" ht="14.4">
-      <c r="A88" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="B88" s="10"/>
-      <c r="C88" s="7" t="s">
-        <v>178</v>
+      <c r="A88" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B88" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>170</v>
       </c>
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
@@ -2367,12 +2722,14 @@
       <c r="I88" s="3"/>
     </row>
     <row r="89" spans="1:9" ht="14.4">
-      <c r="A89" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="B89" s="10"/>
-      <c r="C89" s="7" t="s">
-        <v>178</v>
+      <c r="A89" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B89" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>170</v>
       </c>
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
@@ -2382,12 +2739,14 @@
       <c r="I89" s="3"/>
     </row>
     <row r="90" spans="1:9" ht="14.4">
-      <c r="A90" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="B90" s="10"/>
-      <c r="C90" s="7" t="s">
-        <v>181</v>
+      <c r="A90" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B90" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>173</v>
       </c>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
@@ -2397,12 +2756,14 @@
       <c r="I90" s="3"/>
     </row>
     <row r="91" spans="1:9" ht="14.4">
-      <c r="A91" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="B91" s="10"/>
-      <c r="C91" s="7" t="s">
-        <v>183</v>
+      <c r="A91" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B91" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>175</v>
       </c>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
@@ -2412,12 +2773,14 @@
       <c r="I91" s="3"/>
     </row>
     <row r="92" spans="1:9" ht="14.4">
-      <c r="A92" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="B92" s="10"/>
-      <c r="C92" s="7" t="s">
-        <v>185</v>
+      <c r="A92" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B92" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>177</v>
       </c>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
@@ -2427,12 +2790,14 @@
       <c r="I92" s="3"/>
     </row>
     <row r="93" spans="1:9" ht="14.4">
-      <c r="A93" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="B93" s="10"/>
-      <c r="C93" s="7" t="s">
-        <v>187</v>
+      <c r="A93" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B93" s="15" t="s">
+        <v>257</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>179</v>
       </c>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
@@ -2442,23 +2807,35 @@
       <c r="I93" s="3"/>
     </row>
     <row r="94" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A94" s="10" t="s">
-        <v>188</v>
+      <c r="A94" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B94" s="15" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A95" s="10" t="s">
-        <v>189</v>
+      <c r="A95" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B95" s="15" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A96" s="10" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A97" s="10" t="s">
-        <v>191</v>
+      <c r="A96" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B96" s="15" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A97" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="B97" s="15" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix T and P values
</commit_message>
<xml_diff>
--- a/python_script_preprocessing/Inputtypesfilesspreadsheet.xlsx
+++ b/python_script_preprocessing/Inputtypesfilesspreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arithmethic-parser-\python_script_preprocessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E44A0D-6327-4E62-A874-8ED341C9668C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C09253-A9E0-40F9-96CD-7109B1AFA73F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="252">
   <si>
     <t>Input</t>
   </si>
@@ -28,15 +28,9 @@
     <t>output</t>
   </si>
   <si>
-    <t>current compileing</t>
-  </si>
-  <si>
     <t>Fraction(20, 1)'</t>
   </si>
   <si>
-    <t>Fraction(20,1)</t>
-  </si>
-  <si>
     <t>20.'</t>
   </si>
   <si>
@@ -46,9 +40,6 @@
     <t>Fraction(4, 5)</t>
   </si>
   <si>
-    <t>Fraction (4,5)</t>
-  </si>
-  <si>
     <t>20hz</t>
   </si>
   <si>
@@ -61,15 +52,9 @@
     <t>Fraction(20000000, 1)</t>
   </si>
   <si>
-    <t>Fraction (2000000,1)</t>
-  </si>
-  <si>
     <t>20Mhz</t>
   </si>
   <si>
-    <t>Fraction(20000000,1)</t>
-  </si>
-  <si>
     <t>20MHz</t>
   </si>
   <si>
@@ -145,18 +130,12 @@
     <t>Fraction(2, 1)</t>
   </si>
   <si>
-    <t>Fraction(2/1)</t>
-  </si>
-  <si>
     <t>-5/-2+(8/5)*2'</t>
   </si>
   <si>
     <t>Fraction(57, 10)</t>
   </si>
   <si>
-    <t>Fraction(-12/1)</t>
-  </si>
-  <si>
     <t>Fraction(41, 10)</t>
   </si>
   <si>
@@ -178,9 +157,6 @@
     <t>Fraction(1201, 20)</t>
   </si>
   <si>
-    <t>Fraction(0/1687306305536)</t>
-  </si>
-  <si>
     <t>((.3*.5-.1+6))/(.1)</t>
   </si>
   <si>
@@ -193,9 +169,6 @@
     <t>Fraction(1280000000000001, 400000000000000)</t>
   </si>
   <si>
-    <t>1281/400000000</t>
-  </si>
-  <si>
     <t>2y/1y'</t>
   </si>
   <si>
@@ -205,9 +178,6 @@
     <t>Fraction(1430511474609374976, 4768371582031)</t>
   </si>
   <si>
-    <t>Fraction('2748779069444/96')</t>
-  </si>
-  <si>
     <t>3y*3Y'</t>
   </si>
   <si>
@@ -251,9 +221,6 @@
   </si>
   <si>
     <t>112234563/8989k'</t>
-  </si>
-  <si>
-    <t>Fraction(0/1774035337216')</t>
   </si>
   <si>
     <t>112234563f/8989a</t>
@@ -848,7 +815,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -865,12 +832,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor rgb="FF00B0F0"/>
       </patternFill>
     </fill>
     <fill>
@@ -892,7 +853,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -907,11 +868,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1133,1718 +1093,1544 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I97"/>
+  <dimension ref="A1:H97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="23.33203125" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="16"/>
+    <col min="2" max="2" width="8.88671875" style="14"/>
     <col min="3" max="3" width="44.33203125" customWidth="1"/>
-    <col min="4" max="4" width="47.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
+      <c r="D1" s="3" t="s">
+        <v>250</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>262</v>
-      </c>
+        <v>251</v>
+      </c>
+      <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1">
       <c r="A2" s="4">
         <v>20</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>184</v>
+      <c r="B2" s="13" t="s">
+        <v>173</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>4</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="7"/>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1">
+      <c r="G2" s="6"/>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>184</v>
+        <v>3</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>173</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>3</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>185</v>
+        <v>4</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>174</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>8</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1">
       <c r="A5" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>184</v>
+        <v>6</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>173</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>10</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1">
       <c r="A6" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>186</v>
+        <v>8</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>175</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>13</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1">
       <c r="A7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>186</v>
+        <v>10</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>175</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>15</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1">
       <c r="A8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>186</v>
+        <v>11</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>175</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>17</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>186</v>
+        <v>13</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>175</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>17</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1">
       <c r="A10" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>187</v>
+        <v>14</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>176</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1">
       <c r="A11" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>188</v>
+        <v>16</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>177</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>189</v>
+        <v>18</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>178</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>190</v>
+        <v>20</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>179</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="14" spans="1:8" ht="15.75" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>191</v>
+        <v>22</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>180</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="15" spans="1:8" ht="15.75" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>192</v>
+        <v>23</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>181</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>29</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="16" spans="1:8" ht="15.75" customHeight="1">
       <c r="A16" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>193</v>
+        <v>25</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>182</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>31</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="17" spans="1:8" ht="15.75" customHeight="1">
       <c r="A17" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>191</v>
+        <v>22</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>180</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="18" spans="1:8" ht="15.75" customHeight="1">
       <c r="A18" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>193</v>
+        <v>27</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>182</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>31</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="19" spans="1:8" ht="15.75" customHeight="1">
       <c r="A19" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>194</v>
+        <v>28</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>183</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>34</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="20" spans="1:8" ht="15.75" customHeight="1">
       <c r="A20" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>195</v>
+        <v>30</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>184</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>34</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="21" spans="1:8" ht="15.75" customHeight="1">
       <c r="A21" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>196</v>
+        <v>31</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>185</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>37</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="22" spans="1:8" ht="15.75" customHeight="1">
       <c r="A22" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>196</v>
+        <v>33</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>185</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>37</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="23" spans="1:8" ht="15.75" customHeight="1">
       <c r="A23" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>197</v>
+        <v>34</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>41</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="24" spans="1:8" ht="15.75" customHeight="1">
       <c r="A24" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>198</v>
+        <v>36</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>187</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>44</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="25" spans="1:8" ht="15.75" customHeight="1">
       <c r="A25" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>194</v>
+        <v>28</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>183</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>45</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="26" spans="1:8" ht="15.75" customHeight="1">
       <c r="A26" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>199</v>
+        <v>39</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>188</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>47</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="27" spans="1:8" ht="15.75" customHeight="1">
       <c r="A27" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>198</v>
+        <v>41</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>187</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>43</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-    </row>
-    <row r="28" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="28" spans="1:8" ht="15.75" customHeight="1">
       <c r="A28" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>198</v>
+        <v>42</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>187</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>43</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-    </row>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="29" spans="1:8" ht="15.75" customHeight="1">
       <c r="A29" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>258</v>
+        <v>43</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>247</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>52</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="30" spans="1:8" ht="15.75" customHeight="1">
       <c r="A30" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>201</v>
+        <v>45</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>190</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>52</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-    </row>
-    <row r="31" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="31" spans="1:8" ht="15.75" customHeight="1">
       <c r="A31" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>202</v>
+        <v>47</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>191</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>57</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-    </row>
-    <row r="32" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="32" spans="1:8" ht="15.75" customHeight="1">
       <c r="A32" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>197</v>
+        <v>49</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>40</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-    </row>
-    <row r="33" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="33" spans="1:8" ht="15.75" customHeight="1">
       <c r="A33" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>203</v>
+        <v>50</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>192</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" s="13" t="s">
-        <v>61</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-    </row>
-    <row r="34" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="34" spans="1:8" ht="15.75" customHeight="1">
       <c r="A34" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>204</v>
+        <v>52</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>193</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>63</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-    </row>
-    <row r="35" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="35" spans="1:8" ht="15.75" customHeight="1">
       <c r="A35" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>205</v>
+        <v>54</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>194</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D35" s="13" t="s">
-        <v>52</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-    </row>
-    <row r="36" spans="1:9" ht="14.4">
+    </row>
+    <row r="36" spans="1:8" ht="14.4">
       <c r="A36" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>206</v>
+        <v>56</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>195</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>52</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-    </row>
-    <row r="37" spans="1:9" ht="14.4">
+    </row>
+    <row r="37" spans="1:8" ht="14.4">
       <c r="A37" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>207</v>
+        <v>58</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>196</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D37" s="13" t="s">
-        <v>52</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-    </row>
-    <row r="38" spans="1:9" ht="14.4">
+    </row>
+    <row r="38" spans="1:8" ht="14.4">
       <c r="A38" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>208</v>
+        <v>60</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>197</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-    </row>
-    <row r="39" spans="1:9" ht="14.4">
+    </row>
+    <row r="39" spans="1:8" ht="14.4">
       <c r="A39" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>194</v>
+        <v>62</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>183</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-    </row>
-    <row r="40" spans="1:9" ht="14.4">
+    </row>
+    <row r="40" spans="1:8" ht="14.4">
       <c r="A40" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="B40" s="15" t="s">
-        <v>259</v>
+        <v>63</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>248</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D40" s="13" t="s">
-        <v>75</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-    </row>
-    <row r="41" spans="1:9" ht="14.4">
+    </row>
+    <row r="41" spans="1:8" ht="14.4">
       <c r="A41" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="B41" s="15" t="s">
-        <v>209</v>
+        <v>66</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>198</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>77</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-    </row>
-    <row r="42" spans="1:9" ht="14.4">
+    </row>
+    <row r="42" spans="1:8" ht="14.4">
       <c r="A42" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>210</v>
+        <v>67</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>199</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>77</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-    </row>
-    <row r="43" spans="1:9" ht="14.4">
+    </row>
+    <row r="43" spans="1:8" ht="14.4">
       <c r="A43" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>211</v>
+        <v>69</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>200</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>81</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-    </row>
-    <row r="44" spans="1:9" ht="14.4">
-      <c r="A44" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B44" s="15" t="s">
-        <v>212</v>
+    </row>
+    <row r="44" spans="1:8" ht="14.4">
+      <c r="A44" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>201</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>83</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-    </row>
-    <row r="45" spans="1:9" ht="14.4">
+    </row>
+    <row r="45" spans="1:8" ht="14.4">
       <c r="A45" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>213</v>
+        <v>73</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>202</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>85</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
-    </row>
-    <row r="46" spans="1:9" ht="14.4">
+    </row>
+    <row r="46" spans="1:8" ht="14.4">
       <c r="A46" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="B46" s="15" t="s">
-        <v>214</v>
+        <v>75</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>203</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
-    </row>
-    <row r="47" spans="1:9" ht="14.4">
+    </row>
+    <row r="47" spans="1:8" ht="14.4">
       <c r="A47" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="B47" s="15" t="s">
-        <v>215</v>
+        <v>77</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>204</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-    </row>
-    <row r="48" spans="1:9" ht="14.4">
+    </row>
+    <row r="48" spans="1:8" ht="14.4">
       <c r="A48" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B48" s="15" t="s">
-        <v>216</v>
+        <v>79</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>205</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
-    </row>
-    <row r="49" spans="1:9" ht="14.4">
+    </row>
+    <row r="49" spans="1:8" ht="14.4">
       <c r="A49" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="B49" s="15" t="s">
-        <v>217</v>
+        <v>81</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>206</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-    </row>
-    <row r="50" spans="1:9" ht="14.4">
+    </row>
+    <row r="50" spans="1:8" ht="14.4">
       <c r="A50" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>218</v>
+        <v>83</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>207</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
-    </row>
-    <row r="51" spans="1:9" ht="14.4">
+    </row>
+    <row r="51" spans="1:8" ht="14.4">
       <c r="A51" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="B51" s="15" t="s">
-        <v>219</v>
+        <v>85</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>208</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-    </row>
-    <row r="52" spans="1:9" ht="14.4">
+    </row>
+    <row r="52" spans="1:8" ht="14.4">
       <c r="A52" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="B52" s="15" t="s">
-        <v>220</v>
+        <v>87</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>209</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
-    </row>
-    <row r="53" spans="1:9" ht="14.4">
+    </row>
+    <row r="53" spans="1:8" ht="14.4">
       <c r="A53" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="B53" s="15" t="s">
-        <v>221</v>
+        <v>89</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>210</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
-    </row>
-    <row r="54" spans="1:9" ht="14.4">
+    </row>
+    <row r="54" spans="1:8" ht="14.4">
       <c r="A54" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="B54" s="15" t="s">
-        <v>222</v>
+        <v>91</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>211</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>103</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="D54" s="3"/>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
-    </row>
-    <row r="55" spans="1:9" ht="14.4">
+    </row>
+    <row r="55" spans="1:8" ht="14.4">
       <c r="A55" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="B55" s="15" t="s">
-        <v>223</v>
+        <v>93</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>212</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D55" s="6" t="s">
-        <v>105</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="D55" s="3"/>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
-      <c r="I55" s="3"/>
-    </row>
-    <row r="56" spans="1:9" ht="14.4">
+    </row>
+    <row r="56" spans="1:8" ht="14.4">
       <c r="A56" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="B56" s="15" t="s">
-        <v>200</v>
+        <v>95</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>189</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
-      <c r="I56" s="3"/>
-    </row>
-    <row r="57" spans="1:9" ht="14.4">
+    </row>
+    <row r="57" spans="1:8" ht="14.4">
       <c r="A57" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="B57" s="15" t="s">
-        <v>224</v>
+        <v>97</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>213</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
-      <c r="I57" s="3"/>
-    </row>
-    <row r="58" spans="1:9" ht="14.4">
+    </row>
+    <row r="58" spans="1:8" ht="14.4">
       <c r="A58" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="B58" s="15" t="s">
-        <v>225</v>
+        <v>99</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>214</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
-      <c r="I58" s="3"/>
-    </row>
-    <row r="59" spans="1:9" ht="14.4">
+    </row>
+    <row r="59" spans="1:8" ht="14.4">
       <c r="A59" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="B59" s="15" t="s">
-        <v>226</v>
+        <v>101</v>
+      </c>
+      <c r="B59" s="13" t="s">
+        <v>215</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
-      <c r="I59" s="3"/>
-    </row>
-    <row r="60" spans="1:9" ht="14.4">
+    </row>
+    <row r="60" spans="1:8" ht="14.4">
       <c r="A60" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="B60" s="15" t="s">
-        <v>227</v>
+        <v>103</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>216</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
-      <c r="I60" s="3"/>
-    </row>
-    <row r="61" spans="1:9" ht="14.4">
+    </row>
+    <row r="61" spans="1:8" ht="14.4">
       <c r="A61" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="B61" s="15" t="s">
-        <v>228</v>
+        <v>105</v>
+      </c>
+      <c r="B61" s="13" t="s">
+        <v>217</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
-      <c r="I61" s="3"/>
-    </row>
-    <row r="62" spans="1:9" ht="14.4">
+    </row>
+    <row r="62" spans="1:8" ht="14.4">
       <c r="A62" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B62" s="15" t="s">
-        <v>229</v>
+        <v>107</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>218</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
-      <c r="I62" s="3"/>
-    </row>
-    <row r="63" spans="1:9" ht="14.4">
+    </row>
+    <row r="63" spans="1:8" ht="14.4">
       <c r="A63" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B63" s="15" t="s">
-        <v>230</v>
+        <v>109</v>
+      </c>
+      <c r="B63" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
-      <c r="I63" s="3"/>
-    </row>
-    <row r="64" spans="1:9" ht="14.4">
+    </row>
+    <row r="64" spans="1:8" ht="14.4">
       <c r="A64" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="B64" s="15" t="s">
-        <v>200</v>
+        <v>101</v>
+      </c>
+      <c r="B64" s="13" t="s">
+        <v>189</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
-      <c r="I64" s="3"/>
-    </row>
-    <row r="65" spans="1:9" ht="14.4">
+    </row>
+    <row r="65" spans="1:8" ht="14.4">
       <c r="A65" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="B65" s="15" t="s">
-        <v>231</v>
+        <v>112</v>
+      </c>
+      <c r="B65" s="13" t="s">
+        <v>220</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
-      <c r="I65" s="3"/>
-    </row>
-    <row r="66" spans="1:9" ht="14.4">
+    </row>
+    <row r="66" spans="1:8" ht="14.4">
       <c r="A66" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="B66" s="15" t="s">
-        <v>232</v>
+        <v>114</v>
+      </c>
+      <c r="B66" s="13" t="s">
+        <v>221</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
-      <c r="I66" s="3"/>
-    </row>
-    <row r="67" spans="1:9" ht="14.4">
+    </row>
+    <row r="67" spans="1:8" ht="14.4">
       <c r="A67" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="B67" s="15" t="s">
-        <v>233</v>
+        <v>116</v>
+      </c>
+      <c r="B67" s="13" t="s">
+        <v>222</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
-      <c r="I67" s="3"/>
-    </row>
-    <row r="68" spans="1:9" ht="14.4">
+    </row>
+    <row r="68" spans="1:8" ht="14.4">
       <c r="A68" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B68" s="15" t="s">
-        <v>234</v>
+        <v>118</v>
+      </c>
+      <c r="B68" s="13" t="s">
+        <v>223</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
-      <c r="I68" s="3"/>
-    </row>
-    <row r="69" spans="1:9" ht="14.4">
+    </row>
+    <row r="69" spans="1:8" ht="14.4">
       <c r="A69" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="B69" s="15" t="s">
-        <v>235</v>
+        <v>120</v>
+      </c>
+      <c r="B69" s="13" t="s">
+        <v>224</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
-      <c r="I69" s="3"/>
-    </row>
-    <row r="70" spans="1:9" ht="14.4">
+    </row>
+    <row r="70" spans="1:8" ht="14.4">
       <c r="A70" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="B70" s="15" t="s">
-        <v>236</v>
+        <v>122</v>
+      </c>
+      <c r="B70" s="13" t="s">
+        <v>225</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
-      <c r="I70" s="3"/>
-    </row>
-    <row r="71" spans="1:9" ht="14.4">
+    </row>
+    <row r="71" spans="1:8" ht="14.4">
       <c r="A71" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="B71" s="15" t="s">
-        <v>237</v>
+        <v>124</v>
+      </c>
+      <c r="B71" s="13" t="s">
+        <v>226</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
-      <c r="I71" s="3"/>
-    </row>
-    <row r="72" spans="1:9" ht="14.4">
+    </row>
+    <row r="72" spans="1:8" ht="14.4">
       <c r="A72" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="B72" s="15" t="s">
-        <v>238</v>
+        <v>126</v>
+      </c>
+      <c r="B72" s="13" t="s">
+        <v>227</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
-      <c r="I72" s="3"/>
-    </row>
-    <row r="73" spans="1:9" ht="14.4">
+    </row>
+    <row r="73" spans="1:8" ht="14.4">
       <c r="A73" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="B73" s="15" t="s">
-        <v>239</v>
+        <v>128</v>
+      </c>
+      <c r="B73" s="13" t="s">
+        <v>228</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
-      <c r="I73" s="3"/>
-    </row>
-    <row r="74" spans="1:9" ht="14.4">
+    </row>
+    <row r="74" spans="1:8" ht="14.4">
       <c r="A74" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="B74" s="15" t="s">
-        <v>240</v>
+        <v>130</v>
+      </c>
+      <c r="B74" s="13" t="s">
+        <v>229</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
-      <c r="I74" s="3"/>
-    </row>
-    <row r="75" spans="1:9" ht="14.4">
-      <c r="A75" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="B75" s="18"/>
-      <c r="C75" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="D75" s="18"/>
-      <c r="E75" s="18"/>
-      <c r="F75" s="18"/>
-      <c r="G75" s="18"/>
-      <c r="H75" s="18"/>
-      <c r="I75" s="3"/>
-    </row>
-    <row r="76" spans="1:9" ht="14.4">
-      <c r="A76" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="B76" s="18"/>
-      <c r="C76" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="D76" s="18"/>
+    </row>
+    <row r="75" spans="1:8" ht="14.4">
+      <c r="A75" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B75" s="17"/>
+      <c r="C75" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="D75" s="17"/>
+      <c r="E75" s="17"/>
+      <c r="F75" s="17"/>
+      <c r="G75" s="17"/>
+      <c r="H75" s="3"/>
+    </row>
+    <row r="76" spans="1:8" ht="14.4">
+      <c r="A76" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="B76" s="17"/>
+      <c r="C76" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="D76" s="3"/>
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
-      <c r="I76" s="3"/>
-    </row>
-    <row r="77" spans="1:9" ht="14.4">
+    </row>
+    <row r="77" spans="1:8" ht="14.4">
       <c r="A77" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="B77" s="15" t="s">
-        <v>241</v>
+        <v>136</v>
+      </c>
+      <c r="B77" s="13" t="s">
+        <v>230</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
-      <c r="I77" s="3"/>
-    </row>
-    <row r="78" spans="1:9" ht="14.4">
+    </row>
+    <row r="78" spans="1:8" ht="14.4">
       <c r="A78" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="B78" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="C78" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="D78" s="18"/>
+        <v>138</v>
+      </c>
+      <c r="B78" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="C78" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="D78" s="3"/>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
-      <c r="I78" s="3"/>
-    </row>
-    <row r="79" spans="1:9" ht="14.4">
+    </row>
+    <row r="79" spans="1:8" ht="14.4">
       <c r="A79" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="B79" s="15" t="s">
-        <v>243</v>
+        <v>140</v>
+      </c>
+      <c r="B79" s="13" t="s">
+        <v>232</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
-      <c r="I79" s="3"/>
-    </row>
-    <row r="80" spans="1:9" ht="14.4">
+    </row>
+    <row r="80" spans="1:8" ht="14.4">
       <c r="A80" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="B80" s="15" t="s">
-        <v>244</v>
+        <v>142</v>
+      </c>
+      <c r="B80" s="13" t="s">
+        <v>233</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
-      <c r="I80" s="3"/>
-    </row>
-    <row r="81" spans="1:9" ht="14.4">
+    </row>
+    <row r="81" spans="1:8" ht="14.4">
       <c r="A81" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="B81" s="15" t="s">
-        <v>245</v>
+        <v>144</v>
+      </c>
+      <c r="B81" s="13" t="s">
+        <v>234</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
-      <c r="I81" s="3"/>
-    </row>
-    <row r="82" spans="1:9" ht="14.4">
+    </row>
+    <row r="82" spans="1:8" ht="14.4">
       <c r="A82" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="B82" s="15" t="s">
-        <v>246</v>
+        <v>146</v>
+      </c>
+      <c r="B82" s="13" t="s">
+        <v>235</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="D82" s="3"/>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
-      <c r="I82" s="3"/>
-    </row>
-    <row r="83" spans="1:9" ht="14.4">
+    </row>
+    <row r="83" spans="1:8" ht="14.4">
       <c r="A83" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="B83" s="15" t="s">
-        <v>247</v>
+        <v>148</v>
+      </c>
+      <c r="B83" s="13" t="s">
+        <v>236</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
       <c r="F83" s="3"/>
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
-      <c r="I83" s="3"/>
-    </row>
-    <row r="84" spans="1:9" ht="14.4">
+    </row>
+    <row r="84" spans="1:8" ht="14.4">
       <c r="A84" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="B84" s="15" t="s">
-        <v>248</v>
+        <v>150</v>
+      </c>
+      <c r="B84" s="13" t="s">
+        <v>237</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
       <c r="G84" s="3"/>
       <c r="H84" s="3"/>
-      <c r="I84" s="3"/>
-    </row>
-    <row r="85" spans="1:9" ht="14.4">
+    </row>
+    <row r="85" spans="1:8" ht="14.4">
       <c r="A85" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="B85" s="15" t="s">
-        <v>249</v>
+        <v>152</v>
+      </c>
+      <c r="B85" s="13" t="s">
+        <v>238</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
-      <c r="I85" s="3"/>
-    </row>
-    <row r="86" spans="1:9" ht="14.4">
+    </row>
+    <row r="86" spans="1:8" ht="14.4">
       <c r="A86" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="B86" s="15" t="s">
-        <v>250</v>
+        <v>154</v>
+      </c>
+      <c r="B86" s="13" t="s">
+        <v>239</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
       <c r="G86" s="3"/>
       <c r="H86" s="3"/>
-      <c r="I86" s="3"/>
-    </row>
-    <row r="87" spans="1:9" ht="14.4">
+    </row>
+    <row r="87" spans="1:8" ht="14.4">
       <c r="A87" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="B87" s="15" t="s">
-        <v>251</v>
+        <v>156</v>
+      </c>
+      <c r="B87" s="13" t="s">
+        <v>240</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
-      <c r="I87" s="3"/>
-    </row>
-    <row r="88" spans="1:9" ht="14.4">
+    </row>
+    <row r="88" spans="1:8" ht="14.4">
       <c r="A88" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="B88" s="15" t="s">
-        <v>252</v>
+        <v>158</v>
+      </c>
+      <c r="B88" s="13" t="s">
+        <v>241</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
-      <c r="I88" s="3"/>
-    </row>
-    <row r="89" spans="1:9" ht="14.4">
+    </row>
+    <row r="89" spans="1:8" ht="14.4">
       <c r="A89" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="B89" s="15" t="s">
-        <v>253</v>
+        <v>160</v>
+      </c>
+      <c r="B89" s="13" t="s">
+        <v>242</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
-      <c r="I89" s="3"/>
-    </row>
-    <row r="90" spans="1:9" ht="14.4">
+    </row>
+    <row r="90" spans="1:8" ht="14.4">
       <c r="A90" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="B90" s="15" t="s">
-        <v>254</v>
+        <v>161</v>
+      </c>
+      <c r="B90" s="13" t="s">
+        <v>243</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
       <c r="G90" s="3"/>
       <c r="H90" s="3"/>
-      <c r="I90" s="3"/>
-    </row>
-    <row r="91" spans="1:9" ht="14.4">
+    </row>
+    <row r="91" spans="1:8" ht="14.4">
       <c r="A91" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="B91" s="15" t="s">
-        <v>255</v>
+        <v>163</v>
+      </c>
+      <c r="B91" s="13" t="s">
+        <v>244</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
       <c r="F91" s="3"/>
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
-      <c r="I91" s="3"/>
-    </row>
-    <row r="92" spans="1:9" ht="14.4">
+    </row>
+    <row r="92" spans="1:8" ht="14.4">
       <c r="A92" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="B92" s="15" t="s">
-        <v>256</v>
+        <v>165</v>
+      </c>
+      <c r="B92" s="13" t="s">
+        <v>245</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
       <c r="F92" s="3"/>
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
-      <c r="I92" s="3"/>
-    </row>
-    <row r="93" spans="1:9" ht="14.4">
+    </row>
+    <row r="93" spans="1:8" ht="14.4">
       <c r="A93" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="B93" s="15" t="s">
-        <v>257</v>
+        <v>167</v>
+      </c>
+      <c r="B93" s="13" t="s">
+        <v>246</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
       <c r="F93" s="3"/>
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
-      <c r="I93" s="3"/>
-    </row>
-    <row r="94" spans="1:9" ht="15.75" customHeight="1">
+    </row>
+    <row r="94" spans="1:8" ht="15.75" customHeight="1">
       <c r="A94" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="B94" s="15" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" ht="15.75" customHeight="1">
+        <v>169</v>
+      </c>
+      <c r="B94" s="13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="15.75" customHeight="1">
       <c r="A95" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="B95" s="15" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" ht="15.75" customHeight="1">
+        <v>170</v>
+      </c>
+      <c r="B95" s="13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="15.75" customHeight="1">
       <c r="A96" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="B96" s="15" t="s">
-        <v>200</v>
+        <v>171</v>
+      </c>
+      <c r="B96" s="13" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="15.75" customHeight="1">
       <c r="A97" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="B97" s="15" t="s">
-        <v>200</v>
+        <v>172</v>
+      </c>
+      <c r="B97" s="13" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="3">
     <mergeCell ref="A75:B75"/>
-    <mergeCell ref="C75:H75"/>
+    <mergeCell ref="C75:G75"/>
     <mergeCell ref="A76:B76"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="C78:D78"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>